<commit_message>
Cambios en primeros y siguientes
</commit_message>
<xml_diff>
--- a/primeros y siguientes.xlsx
+++ b/primeros y siguientes.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9272A45-8729-40A4-9E3B-ADDC2534394D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -14,11 +15,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -176,9 +172,6 @@
     <t xml:space="preserve">INICIO, </t>
   </si>
   <si>
-    <t xml:space="preserve">opsuma, O, </t>
-  </si>
-  <si>
     <t xml:space="preserve">id, num, (, NO, CIERTO, FALSO, </t>
   </si>
   <si>
@@ -198,12 +191,15 @@
   </si>
   <si>
     <t>opmult, Y, opsuma, O, ], oprel, ), ENTONCES, HACER, ;, SINO,</t>
+  </si>
+  <si>
+    <t>id,num,(,NO,CIERTO,FALSO,+,-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -560,23 +556,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" customWidth="1"/>
-    <col min="5" max="5" width="57.5703125" customWidth="1"/>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="38.44140625" customWidth="1"/>
+    <col min="5" max="5" width="57.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" s="3" t="s">
         <v>23</v>
@@ -588,7 +584,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
@@ -602,7 +598,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
@@ -616,7 +612,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>20</v>
       </c>
@@ -630,7 +626,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
@@ -644,7 +640,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
@@ -658,7 +654,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
@@ -672,7 +668,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
@@ -686,7 +682,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
@@ -697,10 +693,10 @@
         <v>36</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
@@ -714,7 +710,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
@@ -728,7 +724,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
@@ -742,7 +738,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
         <v>10</v>
       </c>
@@ -756,7 +752,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
@@ -767,10 +763,10 @@
         <v>26</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
         <v>12</v>
       </c>
@@ -781,10 +777,10 @@
         <v>33</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
@@ -798,7 +794,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="4" t="s">
         <v>14</v>
       </c>
@@ -806,13 +802,13 @@
         <v>24</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="4" t="s">
         <v>42</v>
       </c>
@@ -823,10 +819,10 @@
         <v>43</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
         <v>15</v>
       </c>
@@ -837,12 +833,12 @@
         <v>31</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>25</v>
@@ -851,10 +847,10 @@
         <v>29</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
         <v>16</v>
       </c>
@@ -865,10 +861,10 @@
         <v>27</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
         <v>17</v>
       </c>
@@ -879,10 +875,10 @@
         <v>28</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="4" t="s">
         <v>18</v>
       </c>
@@ -893,10 +889,10 @@
         <v>27</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
         <v>19</v>
       </c>
@@ -907,7 +903,7 @@
         <v>30</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Terminado el analizador sintáctico
</commit_message>
<xml_diff>
--- a/primeros y siguientes.xlsx
+++ b/primeros y siguientes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9272A45-8729-40A4-9E3B-ADDC2534394D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DAA028-ABDA-4EAF-B147-E6FA065A57C0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
   <si>
     <t>decl_var</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>id,num,(,NO,CIERTO,FALSO,+,-</t>
+  </si>
+  <si>
+    <t>id, num, (, NO, CIERTO, FALSO</t>
   </si>
 </sst>
 </file>
@@ -559,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -858,7 +861,7 @@
         <v>24</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>55</v>

</xml_diff>